<commit_message>
automatização da planilha Tr x Td
</commit_message>
<xml_diff>
--- a/Atividade 5/casos_estaveis.xlsx
+++ b/Atividade 5/casos_estaveis.xlsx
@@ -195,16 +195,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="23.96"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -224,7 +224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -247,7 +247,7 @@
         <v>0.00390771777</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -270,7 +270,7 @@
         <v>-0.568921528455</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -293,7 +293,7 @@
         <v>-0.0524671328657009</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -316,7 +316,7 @@
         <v>0.660285859128959</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -339,7 +339,7 @@
         <v>-0.000538950169223414</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -362,7 +362,7 @@
         <v>3.91445034884298E-006</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -385,7 +385,7 @@
         <v>-0.0490983652649243</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -408,7 +408,7 @@
         <v>0.0913682451243075</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -431,7 +431,7 @@
         <v>85.5734717474294</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -454,7 +454,7 @@
         <v>52.5734717474294</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>